<commit_message>
implemented functionality for dynamic template generation
</commit_message>
<xml_diff>
--- a/spreadsheets/test_data.xlsx
+++ b/spreadsheets/test_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/ra1422_ic_ac_uk/Documents/extra work/projects/python/email-client/text_menu/spreadsheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/ra1422_ic_ac_uk/Documents/extra work/projects/python/email-client/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="11_F25DC773A252ABDACC104800D9DD4A9C5ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A11A75F0-1E00-4A62-BAB9-9E843F347668}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="11_F25DC773A252ABDACC104800D9DD4A9C5ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48DC6337-81A1-48A0-B021-D9D5195FB2D5}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="36" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Company name</t>
   </si>
@@ -61,6 +61,15 @@
   </si>
   <si>
     <t>ghi@gmail.com</t>
+  </si>
+  <si>
+    <t>template_to_send</t>
+  </si>
+  <si>
+    <t>test_template.docx</t>
+  </si>
+  <si>
+    <t>test_template_2.txt</t>
   </si>
 </sst>
 </file>
@@ -124,6 +133,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -389,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -400,9 +413,10 @@
     <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="17.109375" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -412,8 +426,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -423,8 +440,11 @@
       <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -434,8 +454,11 @@
       <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -444,6 +467,9 @@
       </c>
       <c r="C4" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented some test files to run the project under to ensure accuracy
</commit_message>
<xml_diff>
--- a/spreadsheets/test_data.xlsx
+++ b/spreadsheets/test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/ra1422_ic_ac_uk/Documents/extra work/projects/python/email-client/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="11_F25DC773A252ABDACC104800D9DD4A9C5ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48DC6337-81A1-48A0-B021-D9D5195FB2D5}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="11_F25DC773A252ABDACC104800D9DD4A9C5ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B71B2CE2-7A61-4EC3-9B38-A0D9FA5AA2E3}"/>
   <bookViews>
     <workbookView xWindow="5760" yWindow="36" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Company name</t>
   </si>
@@ -70,6 +70,18 @@
   </si>
   <si>
     <t>test_template_2.txt</t>
+  </si>
+  <si>
+    <t>Company D</t>
+  </si>
+  <si>
+    <t>AI researcher</t>
+  </si>
+  <si>
+    <t>unknown@gmail.com</t>
+  </si>
+  <si>
+    <t>non_existant_template.pdf</t>
   </si>
 </sst>
 </file>
@@ -402,18 +414,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="17.109375" customWidth="1"/>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -470,6 +482,20 @@
       </c>
       <c r="D4" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -477,6 +503,7 @@
     <hyperlink ref="C2" r:id="rId1" xr:uid="{49F97E77-A62C-4415-8FB2-DF13A8600D23}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{91B0BEC1-8A62-43EF-876F-91BC61995C63}"/>
     <hyperlink ref="C4" r:id="rId3" xr:uid="{BDDAFB56-99BC-4FCF-A390-C9F3AE0EE94A}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{5C3B1271-18D5-4945-8C5D-35C669F7E542}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Integrated email sending into the main menu, now the user can create templates and send them off within the same run of the program
</commit_message>
<xml_diff>
--- a/spreadsheets/test_data.xlsx
+++ b/spreadsheets/test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/ra1422_ic_ac_uk/Documents/extra work/projects/python/email-client/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="11_F25DC773A252ABDACC104800D9DD4A9C5ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B71B2CE2-7A61-4EC3-9B38-A0D9FA5AA2E3}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="11_F25DC773A252ABDACC104800D9DD4A9C5ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1DFDE4DF-926F-44C9-9602-F8FBF5D3F62F}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="36" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5004" yWindow="1032" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Company name</t>
   </si>
@@ -82,6 +82,18 @@
   </si>
   <si>
     <t>non_existant_template.pdf</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>rayanakhtar120330@gmail.com</t>
+  </si>
+  <si>
+    <t>r.ak200330@gmail.com</t>
+  </si>
+  <si>
+    <t>rayan.ak12321@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -414,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -426,9 +438,10 @@
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -441,8 +454,11 @@
       <c r="D1" t="s">
         <v>12</v>
       </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -455,8 +471,11 @@
       <c r="D2" t="s">
         <v>13</v>
       </c>
+      <c r="E2" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -469,8 +488,11 @@
       <c r="D3" t="s">
         <v>14</v>
       </c>
+      <c r="E3" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -483,8 +505,11 @@
       <c r="D4" t="s">
         <v>13</v>
       </c>
+      <c r="E4" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -496,6 +521,9 @@
       </c>
       <c r="D5" t="s">
         <v>18</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -504,6 +532,10 @@
     <hyperlink ref="C3" r:id="rId2" xr:uid="{91B0BEC1-8A62-43EF-876F-91BC61995C63}"/>
     <hyperlink ref="C4" r:id="rId3" xr:uid="{BDDAFB56-99BC-4FCF-A390-C9F3AE0EE94A}"/>
     <hyperlink ref="C5" r:id="rId4" xr:uid="{5C3B1271-18D5-4945-8C5D-35C669F7E542}"/>
+    <hyperlink ref="E2" r:id="rId5" xr:uid="{0DBA0AA4-9DFA-4E0C-973E-01B607D1E0E7}"/>
+    <hyperlink ref="E3" r:id="rId6" xr:uid="{28470FD3-49DB-4EA8-B903-A011AFB7D118}"/>
+    <hyperlink ref="E4" r:id="rId7" xr:uid="{91BDD6F1-2B7E-45EA-B5AE-0A94D9F524B6}"/>
+    <hyperlink ref="E5" r:id="rId8" xr:uid="{E78440E4-9E2F-4099-B340-3509C45A7F87}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Debugging and added comments
</commit_message>
<xml_diff>
--- a/spreadsheets/test_data.xlsx
+++ b/spreadsheets/test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/ra1422_ic_ac_uk/Documents/extra work/projects/python/email-client/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="11_F25DC773A252ABDACC104800D9DD4A9C5ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1DFDE4DF-926F-44C9-9602-F8FBF5D3F62F}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="11_F25DC773A252ABDACC104800D9DD4A9C5ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49BA28B6-77D1-45DD-A8A4-A594BDE50932}"/>
   <bookViews>
     <workbookView xWindow="5004" yWindow="1032" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>Company name</t>
   </si>
@@ -63,9 +63,6 @@
     <t>ghi@gmail.com</t>
   </si>
   <si>
-    <t>template_to_send</t>
-  </si>
-  <si>
     <t>test_template.docx</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
     <t>AI researcher</t>
   </si>
   <si>
-    <t>unknown@gmail.com</t>
-  </si>
-  <si>
     <t>non_existant_template.pdf</t>
   </si>
   <si>
@@ -94,6 +88,30 @@
   </si>
   <si>
     <t>rayan.ak12321@gmail.com</t>
+  </si>
+  <si>
+    <t>Company E</t>
+  </si>
+  <si>
+    <t>Something else</t>
+  </si>
+  <si>
+    <t>some_other_email@gmail.com</t>
+  </si>
+  <si>
+    <t>file_1</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>Software engineering internship</t>
+  </si>
+  <si>
+    <t>Software developer internship</t>
+  </si>
+  <si>
+    <t>data science internship</t>
   </si>
 </sst>
 </file>
@@ -426,22 +444,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -452,13 +471,16 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -469,13 +491,16 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -486,13 +511,16 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -503,27 +531,40 @@
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="C6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -531,11 +572,11 @@
     <hyperlink ref="C2" r:id="rId1" xr:uid="{49F97E77-A62C-4415-8FB2-DF13A8600D23}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{91B0BEC1-8A62-43EF-876F-91BC61995C63}"/>
     <hyperlink ref="C4" r:id="rId3" xr:uid="{BDDAFB56-99BC-4FCF-A390-C9F3AE0EE94A}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{5C3B1271-18D5-4945-8C5D-35C669F7E542}"/>
-    <hyperlink ref="E2" r:id="rId5" xr:uid="{0DBA0AA4-9DFA-4E0C-973E-01B607D1E0E7}"/>
-    <hyperlink ref="E3" r:id="rId6" xr:uid="{28470FD3-49DB-4EA8-B903-A011AFB7D118}"/>
-    <hyperlink ref="E4" r:id="rId7" xr:uid="{91BDD6F1-2B7E-45EA-B5AE-0A94D9F524B6}"/>
-    <hyperlink ref="E5" r:id="rId8" xr:uid="{E78440E4-9E2F-4099-B340-3509C45A7F87}"/>
+    <hyperlink ref="E2" r:id="rId4" xr:uid="{0DBA0AA4-9DFA-4E0C-973E-01B607D1E0E7}"/>
+    <hyperlink ref="E3" r:id="rId5" xr:uid="{28470FD3-49DB-4EA8-B903-A011AFB7D118}"/>
+    <hyperlink ref="E4" r:id="rId6" xr:uid="{91BDD6F1-2B7E-45EA-B5AE-0A94D9F524B6}"/>
+    <hyperlink ref="C6" r:id="rId7" xr:uid="{F473D3A3-A6D8-45FD-8023-DBBAD9373CE5}"/>
+    <hyperlink ref="E6" r:id="rId8" xr:uid="{5B36796B-F14F-440A-98A4-200F019677ED}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>